<commit_message>
la répartition des heures ultra simplifiée
</commit_message>
<xml_diff>
--- a/Divers/Consignes/Répartition_heures.xlsx
+++ b/Divers/Consignes/Répartition_heures.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -49,6 +49,1350 @@
         </r>
       </text>
     </comment>
+    <comment ref="D5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Discussion, modélisation système de sauvegarde et de l'historique d'action</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mise en place du système de sauvegarde</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Création du canevas + création des calques</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+undo/redo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+finition undo-redo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+vérfication état du projet + insertion d'image</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion image + insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + tests</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + préparation présentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Apprentissage JavaFX </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Création de l'interface utilisateur </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Création de l'interface utilisateur </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+outils dessin + fonction modif calque</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+finission de calques</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+vérfication état du projet + insertion d'image</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion image + insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + tests</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + préparation présentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Apprentissage JavaFX </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Création de l'interface utilisateur</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Création de l'interface utilisateur </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+outils dessin + fonction modif calque</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+vérfication état du projet + insertion d'image</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion image + insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + tests</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + préparation présentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Apprentissage JavaFX </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Création de l'interface utilisateur</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Création de l'interface utilisateur </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+outils dessin + fonction modif calque</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+vérfication état du projet + insertion d'image</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion image + insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + tests</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + préparation présentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Discussion, modélisation système de sauvegarde et de l'historique d'action</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mise en place du système de sauvegarde</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Création du canevas + création des calques</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+undo/redo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+vérfication état du projet + insertion d'image</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion image + insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + tests</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + préparation présentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Discussion, modélisation système de sauvegarde et de l'historique d'action</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mise en place du système de sauvegarde</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Création du canevas + création des calques</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+undo/redo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+vérfication état du projet + insertion d'image</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion image + insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+finition insertion forme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + tests</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation + préparation présentation</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -59,21 +1403,6 @@
     <t xml:space="preserve">Contraintes </t>
   </si>
   <si>
-    <t>Développeur 2</t>
-  </si>
-  <si>
-    <t>Développeur 3</t>
-  </si>
-  <si>
-    <t>Développeur 4</t>
-  </si>
-  <si>
-    <t>Développeur 5</t>
-  </si>
-  <si>
-    <t>Développeur 6</t>
-  </si>
-  <si>
     <t>6 développeurs x 90h = 540h au total</t>
   </si>
   <si>
@@ -143,9 +1472,6 @@
     <t>Total [h]</t>
   </si>
   <si>
-    <t>Jean Ziegler</t>
-  </si>
-  <si>
     <t>90 heures de travail par développeur sur l'ensemble du semestre</t>
   </si>
   <si>
@@ -159,13 +1485,31 @@
   </si>
   <si>
     <t>30h / 5 = 6h de travail par semaine et par développeur</t>
+  </si>
+  <si>
+    <t>Benoît Schopfer</t>
+  </si>
+  <si>
+    <t>Adrien Allemand</t>
+  </si>
+  <si>
+    <t>Antoine Rochat</t>
+  </si>
+  <si>
+    <t>James Smith</t>
+  </si>
+  <si>
+    <t>Jérémie Chatillion</t>
+  </si>
+  <si>
+    <t>Loyse Krug</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +1537,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -561,255 +1918,421 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="7" customWidth="1"/>
-    <col min="2" max="17" width="5.33203125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="8.77734375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="7" customWidth="1"/>
+    <col min="2" max="17" width="5.28515625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
     </row>
-    <row r="4" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>8</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>6</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1">
+        <v>9</v>
+      </c>
+      <c r="O5" s="1">
         <v>5.5</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="14"/>
+      <c r="P5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>1.5</v>
+      </c>
       <c r="R5" s="4">
         <f>SUM(B5:Q5)</f>
-        <v>5.5</v>
+        <v>73.5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="14"/>
+      <c r="D6" s="1">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1">
+        <v>5</v>
+      </c>
+      <c r="L6" s="1">
+        <v>6</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1">
+        <v>9</v>
+      </c>
+      <c r="O6" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>1.5</v>
+      </c>
       <c r="R6" s="4">
         <f t="shared" ref="R6:R10" si="0">SUM(B6:Q6)</f>
-        <v>5</v>
+        <v>78.5</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1">
         <v>6.5</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="14"/>
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1">
+        <v>6</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1">
+        <v>9</v>
+      </c>
+      <c r="O7" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="P7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>1.5</v>
+      </c>
       <c r="R7" s="4">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="14"/>
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>8</v>
+      </c>
+      <c r="K8" s="1">
+        <v>5</v>
+      </c>
+      <c r="L8" s="1">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="N8" s="1">
+        <v>9</v>
+      </c>
+      <c r="O8" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>1.5</v>
+      </c>
       <c r="R8" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1">
         <v>6</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="14"/>
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1">
+        <v>8</v>
+      </c>
+      <c r="K9" s="1">
+        <v>5</v>
+      </c>
+      <c r="L9" s="1">
+        <v>6</v>
+      </c>
+      <c r="M9" s="1">
+        <v>6</v>
+      </c>
+      <c r="N9" s="1">
+        <v>9</v>
+      </c>
+      <c r="O9" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>1.5</v>
+      </c>
       <c r="R9" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>80.5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1">
         <v>6</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="14"/>
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4</v>
+      </c>
+      <c r="I10" s="1">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>8</v>
+      </c>
+      <c r="K10" s="1">
+        <v>5</v>
+      </c>
+      <c r="L10" s="1">
+        <v>6</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1">
+        <v>9</v>
+      </c>
+      <c r="O10" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>1.5</v>
+      </c>
       <c r="R10" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>79.5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" s="4">
         <f>SUM(B5:B10)</f>
-        <v>34</v>
+        <v>28.5</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" ref="C11:Q11" si="1">SUM(C5:C10)</f>
@@ -817,115 +2340,115 @@
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="M11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>31.5</v>
       </c>
       <c r="N11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="O11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R11" s="12">
         <f>SUM(R5:R10)</f>
-        <v>34</v>
+        <v>471</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
toujours répartition des heures ultra simplifiées
</commit_message>
<xml_diff>
--- a/Divers/Consignes/Répartition_heures.xlsx
+++ b/Divers/Consignes/Répartition_heures.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,8 +45,23 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-- 3h sur modélisation BD
-- 2h sur schéma UML</t>
+- 3h discussion projet
+- 30 min relecture feuille de présentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Auteur:
+</t>
         </r>
       </text>
     </comment>
@@ -69,7 +85,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Discussion, modélisation système de sauvegarde et de l'historique d'action</t>
+- 4h Discussion 
+- 4h modélisation système de sauvegarde et de l'historique d'action</t>
         </r>
       </text>
     </comment>
@@ -289,6 +306,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="B6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- 2h30 discussion projet
+- 30 min relecture feuille de présentation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D6" authorId="0" shapeId="0">
       <text>
         <r>
@@ -529,6 +571,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="B7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- 2h30 discussion projet
+- 30 min relecture feuille de présentation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D7" authorId="0" shapeId="0">
       <text>
         <r>
@@ -745,6 +812,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- 2h30 discussion projet
+- 30 min relecture feuille de présentation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D8" authorId="0" shapeId="0">
       <text>
         <r>
@@ -961,6 +1053,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- 2h30 discussion projet
+- redaction de la feuille de présentation
+- 30 min relecture feuille de présentation
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D9" authorId="0" shapeId="0">
       <text>
         <r>
@@ -981,7 +1100,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Discussion, modélisation système de sauvegarde et de l'historique d'action</t>
+- 4h Discussion 
+- 4h modélisation système de sauvegarde et de l'historique d'action</t>
         </r>
       </text>
     </comment>
@@ -1177,6 +1297,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="B10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- 2h30 discussion projet
+- 30 min relecture feuille de présentation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D10" authorId="0" shapeId="0">
       <text>
         <r>
@@ -1197,7 +1342,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Discussion, modélisation système de sauvegarde et de l'historique d'action</t>
+- 4h Discussion 
+- 4h modélisation système de sauvegarde et de l'historique d'action</t>
         </r>
       </text>
     </comment>
@@ -1918,7 +2064,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,7 +2148,9 @@
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>3.5</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>8</v>
@@ -2047,8 +2195,8 @@
         <v>1.5</v>
       </c>
       <c r="R5" s="4">
-        <f>SUM(B5:Q5)</f>
-        <v>73.5</v>
+        <f t="shared" ref="R5:R10" si="0">SUM(B5:Q5)</f>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2056,7 +2204,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
@@ -2102,8 +2250,8 @@
         <v>1.5</v>
       </c>
       <c r="R6" s="4">
-        <f t="shared" ref="R6:R10" si="0">SUM(B6:Q6)</f>
-        <v>78.5</v>
+        <f t="shared" si="0"/>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2111,7 +2259,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="1">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
@@ -2158,7 +2306,7 @@
       </c>
       <c r="R7" s="4">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2166,7 +2314,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="1">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
@@ -2213,7 +2361,7 @@
       </c>
       <c r="R8" s="4">
         <f t="shared" si="0"/>
-        <v>79</v>
+        <v>77.5</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2221,7 +2369,7 @@
         <v>33</v>
       </c>
       <c r="B9" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
@@ -2268,7 +2416,7 @@
       </c>
       <c r="R9" s="4">
         <f t="shared" si="0"/>
-        <v>80.5</v>
+        <v>78.5</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2276,7 +2424,7 @@
         <v>34</v>
       </c>
       <c r="B10" s="1">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
@@ -2323,7 +2471,7 @@
       </c>
       <c r="R10" s="4">
         <f t="shared" si="0"/>
-        <v>79.5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2332,7 +2480,7 @@
       </c>
       <c r="B11" s="4">
         <f>SUM(B5:B10)</f>
-        <v>28.5</v>
+        <v>21.5</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" ref="C11:Q11" si="1">SUM(C5:C10)</f>
@@ -2396,7 +2544,7 @@
       </c>
       <c r="R11" s="12">
         <f>SUM(R5:R10)</f>
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>